<commit_message>
16006: Add checklist for SLURM install
Add ClusterID to checklist

Arvados-DCO-1.1-Signed-off-by: Peter Amstutz <peter.amstutz@curii.com>
</commit_message>
<xml_diff>
--- a/doc/install/new_cluster_checklist_AWS.xlsx
+++ b/doc/install/new_cluster_checklist_AWS.xlsx
@@ -20,10 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Arvados install worksheet for AWS
 Use this to collect information about your cloud resources.  You will need this information to configure Arvados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClusterID</t>
   </si>
   <si>
     <t xml:space="preserve">Machines</t>
@@ -240,17 +243,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.71"/>
@@ -285,166 +288,181 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update new cluster checklist to reflect the deprecation of the SSO server.
No issue #

Arvados-DCO-1.1-Signed-off-by: Ward Vandewege <ward@curii.com>
</commit_message>
<xml_diff>
--- a/doc/install/new_cluster_checklist_AWS.xlsx
+++ b/doc/install/new_cluster_checklist_AWS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">Arvados install worksheet for AWS
 Use this to collect information about your cloud resources.  You will need this information to configure Arvados.</t>
@@ -59,22 +59,16 @@
     <t xml:space="preserve">privkey path</t>
   </si>
   <si>
-    <t xml:space="preserve">SSO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app_secret</t>
-  </si>
-  <si>
-    <t xml:space="preserve">google client id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client secret</t>
+    <t xml:space="preserve">Authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentication provider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google / OpenIDConnect / PAM / LDAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">credentials</t>
   </si>
   <si>
     <t xml:space="preserve">S3 storage</t>
@@ -239,27 +233,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -350,44 +342,43 @@
       <c r="A16" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="B16" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>18</v>
+      <c r="A22" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A23" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -396,34 +387,34 @@
         <v>22</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>23</v>
+      <c r="A28" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,33 +427,26 @@
         <v>29</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A39" s="0" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>